<commit_message>
3/23/2024 - 7:07 initial web ready to host
</commit_message>
<xml_diff>
--- a/Migrade_v.1.2/media/excel-files/SF9.xlsx
+++ b/Migrade_v.1.2/media/excel-files/SF9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angelo\Documents\GitHub\ces_migrade\MiGrade\Migrade_v.1.2\media\excel-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544FD085-399C-419B-9EBC-44B86DFBE526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E47D6C1-3212-4FBB-91FD-A3C23691A030}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" tabRatio="865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" tabRatio="865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRONT" sheetId="149" r:id="rId1"/>
@@ -802,7 +802,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -897,7 +897,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -932,15 +931,168 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -957,164 +1109,48 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1126,31 +1162,49 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1164,8 +1218,80 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1190,10 +1316,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1202,124 +1324,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2737,8 +2742,8 @@
   <sheetPr codeName="Sheet128"/>
   <dimension ref="A3:AC50"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" view="pageBreakPreview" topLeftCell="A10" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2761,20 +2766,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:23" ht="12.75" customHeight="1">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
       <c r="O3" s="15"/>
       <c r="P3" s="29"/>
       <c r="Q3" s="15"/>
@@ -2784,7 +2789,7 @@
       <c r="U3" s="17"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1">
-      <c r="A4" s="57"/>
+      <c r="A4" s="92"/>
       <c r="B4" s="27"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -2797,44 +2802,44 @@
       <c r="K4" s="28"/>
       <c r="L4" s="28"/>
       <c r="M4" s="28"/>
-      <c r="O4" s="53"/>
+      <c r="O4" s="100"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="58" t="s">
+      <c r="Q4" s="104" t="s">
         <v>98</v>
       </c>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="104"/>
     </row>
     <row r="5" spans="1:23" ht="15" customHeight="1">
-      <c r="A5" s="57"/>
-      <c r="B5" s="77" t="s">
+      <c r="A5" s="92"/>
+      <c r="B5" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
       <c r="L5" s="28"/>
       <c r="M5" s="28"/>
-      <c r="O5" s="53"/>
+      <c r="O5" s="100"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="59" t="s">
+      <c r="Q5" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="59"/>
+      <c r="R5" s="105"/>
+      <c r="S5" s="105"/>
+      <c r="T5" s="105"/>
+      <c r="U5" s="105"/>
     </row>
     <row r="6" spans="1:23" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="57"/>
+      <c r="A6" s="92"/>
       <c r="B6" s="27"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -2848,19 +2853,19 @@
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
       <c r="N6"/>
-      <c r="O6" s="53"/>
+      <c r="O6" s="100"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="100" t="s">
+      <c r="Q6" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="R6" s="100"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
-      <c r="U6" s="100"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1">
-      <c r="A7" s="61"/>
-      <c r="B7" s="88" t="s">
+      <c r="A7" s="93"/>
+      <c r="B7" s="76" t="s">
         <v>82</v>
       </c>
       <c r="C7" s="64" t="s">
@@ -2896,22 +2901,22 @@
       <c r="M7" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="N7" s="67" t="s">
+      <c r="N7" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="53"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="101" t="s">
+      <c r="O7" s="100"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="R7" s="101"/>
-      <c r="S7" s="101"/>
-      <c r="T7" s="101"/>
-      <c r="U7" s="101"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="50"/>
     </row>
     <row r="8" spans="1:23" ht="11.25" customHeight="1">
-      <c r="A8" s="62"/>
-      <c r="B8" s="89"/>
+      <c r="A8" s="94"/>
+      <c r="B8" s="77"/>
       <c r="C8" s="65"/>
       <c r="D8" s="65"/>
       <c r="E8" s="65"/>
@@ -2923,20 +2928,20 @@
       <c r="K8" s="65"/>
       <c r="L8" s="65"/>
       <c r="M8" s="65"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="102" t="s">
+      <c r="N8" s="97"/>
+      <c r="O8" s="100"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="R8" s="102"/>
-      <c r="S8" s="102"/>
-      <c r="T8" s="102"/>
-      <c r="U8" s="102"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
     </row>
     <row r="9" spans="1:23" ht="3.75" customHeight="1">
-      <c r="A9" s="62"/>
-      <c r="B9" s="89"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="65"/>
       <c r="D9" s="65"/>
       <c r="E9" s="65"/>
@@ -2948,9 +2953,9 @@
       <c r="K9" s="65"/>
       <c r="L9" s="65"/>
       <c r="M9" s="65"/>
-      <c r="N9" s="68"/>
+      <c r="N9" s="97"/>
       <c r="O9" s="17"/>
-      <c r="P9" s="52"/>
+      <c r="P9" s="99"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
@@ -2958,8 +2963,8 @@
       <c r="U9" s="17"/>
     </row>
     <row r="10" spans="1:23" ht="16.5" customHeight="1">
-      <c r="A10" s="62"/>
-      <c r="B10" s="89"/>
+      <c r="A10" s="94"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="65"/>
       <c r="D10" s="65"/>
       <c r="E10" s="65"/>
@@ -2971,18 +2976,18 @@
       <c r="K10" s="65"/>
       <c r="L10" s="65"/>
       <c r="M10" s="65"/>
-      <c r="N10" s="68"/>
+      <c r="N10" s="97"/>
       <c r="O10" s="17"/>
       <c r="P10" s="30"/>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="51"/>
-      <c r="S10" s="51"/>
-      <c r="T10" s="51"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="73"/>
       <c r="U10" s="17"/>
     </row>
     <row r="11" spans="1:23" ht="10.5" customHeight="1">
-      <c r="A11" s="63"/>
-      <c r="B11" s="90"/>
+      <c r="A11" s="95"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
       <c r="E11" s="66"/>
@@ -2994,7 +2999,7 @@
       <c r="K11" s="66"/>
       <c r="L11" s="66"/>
       <c r="M11" s="66"/>
-      <c r="N11" s="69"/>
+      <c r="N11" s="98"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="20"/>
@@ -3004,47 +3009,47 @@
       <c r="U11" s="17"/>
     </row>
     <row r="12" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="94"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="55"/>
       <c r="O12" s="17"/>
       <c r="P12" s="30"/>
-      <c r="Q12" s="49" t="s">
+      <c r="Q12" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="R12" s="49"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="49"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="89"/>
     </row>
     <row r="13" spans="1:23" ht="16.5" customHeight="1">
-      <c r="A13" s="98"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="95"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="56"/>
       <c r="P13" s="20"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
@@ -3054,20 +3059,20 @@
       <c r="W13" s="13"/>
     </row>
     <row r="14" spans="1:23" ht="10.5" customHeight="1">
-      <c r="A14" s="98"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="80"/>
-      <c r="N14" s="95"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="56"/>
       <c r="P14" s="20" t="s">
         <v>108</v>
       </c>
@@ -3079,20 +3084,20 @@
       <c r="V14" s="20"/>
     </row>
     <row r="15" spans="1:23" ht="11.25" customHeight="1">
-      <c r="A15" s="99"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="96"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="57"/>
       <c r="P15" s="20" t="s">
         <v>109</v>
       </c>
@@ -3104,22 +3109,22 @@
       <c r="V15" s="20"/>
     </row>
     <row r="16" spans="1:23" s="2" customFormat="1" ht="12" customHeight="1">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="82"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82"/>
-      <c r="N16" s="103"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="58"/>
       <c r="P16" s="20" t="s">
         <v>110</v>
       </c>
@@ -3134,20 +3139,20 @@
       <c r="W16" s="20"/>
     </row>
     <row r="17" spans="1:27" ht="15" customHeight="1">
-      <c r="A17" s="98"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="83"/>
-      <c r="N17" s="104"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="59"/>
       <c r="P17" s="20" t="s">
         <v>111</v>
       </c>
@@ -3161,20 +3166,20 @@
       <c r="V17" s="20"/>
     </row>
     <row r="18" spans="1:27" ht="11.25" customHeight="1">
-      <c r="A18" s="98"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="104"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="59"/>
       <c r="P18" s="20" t="s">
         <v>60</v>
       </c>
@@ -3186,20 +3191,20 @@
       <c r="V18" s="20"/>
     </row>
     <row r="19" spans="1:27" ht="11.25" customHeight="1">
-      <c r="A19" s="99"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
-      <c r="M19" s="84"/>
-      <c r="N19" s="105"/>
+      <c r="A19" s="72"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="60"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="18"/>
@@ -3208,46 +3213,46 @@
       <c r="U19" s="7"/>
     </row>
     <row r="20" spans="1:27" ht="11.25" customHeight="1">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="91"/>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="85"/>
-      <c r="K20" s="85"/>
-      <c r="L20" s="85"/>
-      <c r="M20" s="85"/>
-      <c r="N20" s="94"/>
-      <c r="P20" s="55" t="s">
+      <c r="B20" s="79"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="55"/>
+      <c r="P20" s="102" t="s">
         <v>103</v>
       </c>
-      <c r="Q20" s="55"/>
+      <c r="Q20" s="102"/>
       <c r="R20" s="18"/>
       <c r="S20" s="18"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
     </row>
     <row r="21" spans="1:27" ht="11.25" customHeight="1">
-      <c r="A21" s="98"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="86"/>
-      <c r="K21" s="86"/>
-      <c r="L21" s="86"/>
-      <c r="M21" s="86"/>
-      <c r="N21" s="95"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="56"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
@@ -3265,29 +3270,29 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="2" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A22" s="98"/>
-      <c r="B22" s="92"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="86"/>
-      <c r="L22" s="86"/>
-      <c r="M22" s="86"/>
-      <c r="N22" s="95"/>
-      <c r="P22" s="45" t="s">
+      <c r="A22" s="71"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="56"/>
+      <c r="P22" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="Q22" s="47"/>
-      <c r="R22" s="47"/>
-      <c r="S22" s="47"/>
-      <c r="T22" s="47"/>
-      <c r="U22" s="47"/>
-      <c r="V22" s="47"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
+      <c r="T22" s="46"/>
+      <c r="U22" s="46"/>
+      <c r="V22" s="46"/>
       <c r="X22" s="2" t="s">
         <v>59</v>
       </c>
@@ -3297,29 +3302,29 @@
       </c>
     </row>
     <row r="23" spans="1:27" ht="11.25" customHeight="1">
-      <c r="A23" s="98"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="86"/>
-      <c r="M23" s="86"/>
-      <c r="N23" s="95"/>
-      <c r="P23" s="46" t="s">
+      <c r="A23" s="71"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="56"/>
+      <c r="P23" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="47"/>
-      <c r="S23" s="47"/>
-      <c r="T23" s="47"/>
-      <c r="U23" s="47"/>
-      <c r="V23" s="47"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="46"/>
+      <c r="V23" s="46"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2" t="s">
         <v>61</v>
@@ -3332,29 +3337,29 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" s="2" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A24" s="99"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="96"/>
-      <c r="P24" s="46" t="s">
+      <c r="A24" s="72"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="57"/>
+      <c r="P24" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="47"/>
-      <c r="S24" s="47"/>
-      <c r="T24" s="47"/>
-      <c r="U24" s="47"/>
-      <c r="V24" s="47"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="46"/>
+      <c r="U24" s="46"/>
+      <c r="V24" s="46"/>
       <c r="X24" s="2" t="s">
         <v>60</v>
       </c>
@@ -3376,15 +3381,15 @@
       <c r="K25" s="25"/>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
-      <c r="P25" s="72" t="s">
+      <c r="P25" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="Q25" s="72"/>
-      <c r="R25" s="72"/>
-      <c r="S25" s="47"/>
-      <c r="T25" s="47"/>
-      <c r="U25" s="47"/>
-      <c r="V25" s="47"/>
+      <c r="Q25" s="84"/>
+      <c r="R25" s="84"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="46"/>
+      <c r="U25" s="46"/>
+      <c r="V25" s="46"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2" t="s">
         <v>63</v>
@@ -3397,13 +3402,13 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
-      <c r="P26" s="72"/>
-      <c r="Q26" s="72"/>
-      <c r="R26" s="72"/>
-      <c r="S26" s="48"/>
-      <c r="T26" s="71"/>
-      <c r="U26" s="71"/>
-      <c r="V26" s="71"/>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="83"/>
+      <c r="U26" s="83"/>
+      <c r="V26" s="83"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2" t="s">
         <v>64</v>
@@ -3416,15 +3421,15 @@
       <c r="AA26" s="2"/>
     </row>
     <row r="27" spans="1:27" s="8" customFormat="1" ht="12.75" customHeight="1">
-      <c r="P27" s="51"/>
-      <c r="Q27" s="51"/>
-      <c r="R27" s="51"/>
+      <c r="P27" s="73"/>
+      <c r="Q27" s="73"/>
+      <c r="R27" s="73"/>
       <c r="S27" s="14"/>
-      <c r="T27" s="51" t="s">
+      <c r="T27" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="U27" s="51"/>
-      <c r="V27" s="51"/>
+      <c r="U27" s="73"/>
+      <c r="V27" s="73"/>
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
@@ -3432,25 +3437,25 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15" customHeight="1">
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="74"/>
-      <c r="L28" s="74"/>
-      <c r="M28" s="74"/>
-      <c r="P28" s="51" t="s">
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="P28" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
+      <c r="Q28" s="73"/>
+      <c r="R28" s="73"/>
       <c r="S28" s="21"/>
       <c r="W28" s="2"/>
       <c r="X28" s="2"/>
@@ -3474,30 +3479,30 @@
       <c r="O29" s="3"/>
     </row>
     <row r="30" spans="1:27" s="2" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A30" s="76" t="s">
+      <c r="A30" s="90" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
       <c r="O30" s="3"/>
-      <c r="Q30" s="49" t="s">
+      <c r="Q30" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="49"/>
-      <c r="U30" s="49"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="89"/>
+      <c r="T30" s="89"/>
+      <c r="U30" s="89"/>
     </row>
     <row r="31" spans="1:27" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="O31" s="3"/>
@@ -3515,34 +3520,34 @@
       <c r="AA31" s="4"/>
     </row>
     <row r="32" spans="1:27" ht="18" customHeight="1">
-      <c r="A32" s="70" t="s">
+      <c r="A32" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="70"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="70"/>
-      <c r="N32" s="70"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="50" t="s">
+      <c r="P32" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="75" t="s">
+      <c r="Q32" s="87"/>
+      <c r="R32" s="87"/>
+      <c r="S32" s="87"/>
+      <c r="T32" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="U32" s="75"/>
-      <c r="V32" s="75"/>
+      <c r="U32" s="88"/>
+      <c r="V32" s="88"/>
       <c r="W32" s="9"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
@@ -3551,15 +3556,15 @@
     </row>
     <row r="33" spans="1:29" ht="18" customHeight="1">
       <c r="O33" s="1"/>
-      <c r="P33" s="75" t="s">
+      <c r="P33" s="88" t="s">
         <v>115</v>
       </c>
-      <c r="Q33" s="75"/>
-      <c r="R33" s="75"/>
-      <c r="S33" s="75"/>
-      <c r="T33" s="75"/>
-      <c r="U33" s="75"/>
-      <c r="V33" s="75"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="88"/>
+      <c r="S33" s="88"/>
+      <c r="T33" s="88"/>
+      <c r="U33" s="88"/>
+      <c r="V33" s="88"/>
       <c r="W33" s="3"/>
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
@@ -3598,25 +3603,25 @@
       <c r="AA35" s="5"/>
     </row>
     <row r="36" spans="1:29" ht="12" customHeight="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="82" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="70"/>
-      <c r="L36" s="70"/>
-      <c r="M36" s="70"/>
-      <c r="N36" s="70"/>
-      <c r="T36" s="56"/>
-      <c r="U36" s="56"/>
-      <c r="V36" s="56"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="82"/>
+      <c r="N36" s="82"/>
+      <c r="T36" s="103"/>
+      <c r="U36" s="103"/>
+      <c r="V36" s="103"/>
       <c r="W36" s="3"/>
       <c r="X36" s="9"/>
       <c r="Y36" s="9"/>
@@ -3624,15 +3629,15 @@
       <c r="AA36" s="9"/>
     </row>
     <row r="37" spans="1:29" ht="14.25" customHeight="1">
-      <c r="P37" s="54"/>
-      <c r="Q37" s="54"/>
-      <c r="R37" s="54"/>
+      <c r="P37" s="101"/>
+      <c r="Q37" s="101"/>
+      <c r="R37" s="101"/>
       <c r="S37" s="9"/>
-      <c r="T37" s="51" t="s">
+      <c r="T37" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="U37" s="51"/>
-      <c r="V37" s="51"/>
+      <c r="U37" s="73"/>
+      <c r="V37" s="73"/>
       <c r="W37" s="2"/>
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
@@ -3642,27 +3647,27 @@
       <c r="AC37" s="7"/>
     </row>
     <row r="38" spans="1:29" ht="13.5" customHeight="1">
-      <c r="A38" s="70" t="s">
+      <c r="A38" s="82" t="s">
         <v>121</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="70"/>
-      <c r="M38" s="70"/>
-      <c r="N38" s="70"/>
-      <c r="P38" s="56" t="s">
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="P38" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="56"/>
+      <c r="Q38" s="103"/>
+      <c r="R38" s="103"/>
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
@@ -3679,13 +3684,13 @@
       <c r="AC39" s="3"/>
     </row>
     <row r="40" spans="1:29" s="2" customFormat="1" ht="12" customHeight="1">
-      <c r="Q40" s="49" t="s">
+      <c r="Q40" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="R40" s="49"/>
-      <c r="S40" s="49"/>
-      <c r="T40" s="49"/>
-      <c r="U40" s="49"/>
+      <c r="R40" s="89"/>
+      <c r="S40" s="89"/>
+      <c r="T40" s="89"/>
+      <c r="U40" s="89"/>
       <c r="V40" s="4"/>
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
@@ -3721,15 +3726,15 @@
       <c r="AC42" s="1"/>
     </row>
     <row r="43" spans="1:29" ht="18">
-      <c r="P43" s="50" t="s">
+      <c r="P43" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="Q43" s="50"/>
-      <c r="R43" s="50"/>
-      <c r="S43" s="50"/>
-      <c r="T43" s="57"/>
-      <c r="U43" s="57"/>
-      <c r="V43" s="57"/>
+      <c r="Q43" s="87"/>
+      <c r="R43" s="87"/>
+      <c r="S43" s="87"/>
+      <c r="T43" s="92"/>
+      <c r="U43" s="92"/>
+      <c r="V43" s="92"/>
       <c r="W43" s="16"/>
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
@@ -3741,11 +3746,11 @@
     <row r="44" spans="1:29" ht="18">
       <c r="P44" s="12"/>
       <c r="S44" s="18"/>
-      <c r="T44" s="51" t="s">
+      <c r="T44" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="U44" s="51"/>
-      <c r="V44" s="51"/>
+      <c r="U44" s="73"/>
+      <c r="V44" s="73"/>
       <c r="W44" s="23"/>
       <c r="X44" s="16"/>
       <c r="Y44" s="16"/>
@@ -3798,6 +3803,81 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="91">
+    <mergeCell ref="Q40:U40"/>
+    <mergeCell ref="P43:S43"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="O4:O8"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="T27:V27"/>
+    <mergeCell ref="Q12:U12"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="T36:V36"/>
+    <mergeCell ref="T37:V37"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="T43:V43"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="N7:N11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="A36:N36"/>
+    <mergeCell ref="A38:N38"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="T26:V26"/>
+    <mergeCell ref="P25:R26"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="P32:S32"/>
+    <mergeCell ref="T32:V32"/>
+    <mergeCell ref="P33:V33"/>
+    <mergeCell ref="Q30:U30"/>
+    <mergeCell ref="A30:N30"/>
+    <mergeCell ref="A32:N32"/>
+    <mergeCell ref="T44:V44"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="N20:N24"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="J20:J24"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="M20:M24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
     <mergeCell ref="Q6:U6"/>
     <mergeCell ref="Q7:U7"/>
     <mergeCell ref="Q8:U8"/>
@@ -3814,81 +3894,6 @@
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="K7:K11"/>
     <mergeCell ref="L7:L11"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="N20:N24"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="J20:J24"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="M20:M24"/>
-    <mergeCell ref="T44:V44"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="A36:N36"/>
-    <mergeCell ref="A38:N38"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="T26:V26"/>
-    <mergeCell ref="P25:R26"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="P32:S32"/>
-    <mergeCell ref="T32:V32"/>
-    <mergeCell ref="P33:V33"/>
-    <mergeCell ref="Q30:U30"/>
-    <mergeCell ref="A30:N30"/>
-    <mergeCell ref="A32:N32"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="N7:N11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="M7:M11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="Q40:U40"/>
-    <mergeCell ref="P43:S43"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="P7:P9"/>
-    <mergeCell ref="O4:O8"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="T27:V27"/>
-    <mergeCell ref="Q12:U12"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="T36:V36"/>
-    <mergeCell ref="T37:V37"/>
-    <mergeCell ref="P38:R38"/>
-    <mergeCell ref="T43:V43"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="Q5:U5"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3903,8 +3908,8 @@
   <sheetPr codeName="Sheet127"/>
   <dimension ref="A3:AC29"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3930,45 +3935,45 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:29" ht="18" customHeight="1">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
-      <c r="Q3" s="122"/>
-      <c r="R3" s="122"/>
-      <c r="S3" s="122"/>
-      <c r="U3" s="123" t="s">
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="110"/>
+      <c r="N3" s="110"/>
+      <c r="O3" s="110"/>
+      <c r="P3" s="110"/>
+      <c r="Q3" s="110"/>
+      <c r="R3" s="110"/>
+      <c r="S3" s="110"/>
+      <c r="U3" s="164" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="123"/>
-      <c r="W3" s="123"/>
-      <c r="X3" s="123"/>
-      <c r="Y3" s="123"/>
-      <c r="Z3" s="123"/>
-      <c r="AA3" s="123"/>
-      <c r="AB3" s="123"/>
+      <c r="V3" s="164"/>
+      <c r="W3" s="164"/>
+      <c r="X3" s="164"/>
+      <c r="Y3" s="164"/>
+      <c r="Z3" s="164"/>
+      <c r="AA3" s="164"/>
+      <c r="AB3" s="164"/>
     </row>
     <row r="4" spans="1:29" ht="17.25" customHeight="1"/>
     <row r="5" spans="1:29" ht="15" customHeight="1">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="165" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="124"/>
-      <c r="C5" s="124"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="165"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
@@ -3979,37 +3984,37 @@
       <c r="K5" s="33"/>
       <c r="L5" s="33"/>
       <c r="M5" s="33"/>
-      <c r="N5" s="125" t="s">
+      <c r="N5" s="166" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="125"/>
-      <c r="P5" s="125"/>
-      <c r="Q5" s="126"/>
-      <c r="R5" s="127" t="s">
+      <c r="O5" s="166"/>
+      <c r="P5" s="166"/>
+      <c r="Q5" s="167"/>
+      <c r="R5" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="129" t="s">
+      <c r="S5" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="125" t="s">
+      <c r="U5" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="125" t="s">
+      <c r="V5" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="W5" s="125"/>
-      <c r="X5" s="125"/>
-      <c r="Y5" s="125" t="s">
+      <c r="W5" s="166"/>
+      <c r="X5" s="166"/>
+      <c r="Y5" s="166" t="s">
         <v>12</v>
       </c>
-      <c r="Z5" s="125"/>
-      <c r="AA5" s="125"/>
-      <c r="AB5" s="125"/>
+      <c r="Z5" s="166"/>
+      <c r="AA5" s="166"/>
+      <c r="AB5" s="166"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1">
-      <c r="A6" s="124"/>
-      <c r="B6" s="124"/>
-      <c r="C6" s="124"/>
+      <c r="A6" s="165"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
       <c r="D6" s="33"/>
       <c r="E6" s="33" t="s">
         <v>72</v>
@@ -4038,43 +4043,43 @@
       <c r="M6" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="N6" s="44">
+      <c r="N6" s="43">
         <v>1</v>
       </c>
-      <c r="O6" s="44">
+      <c r="O6" s="43">
         <v>2</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="43">
         <v>3</v>
       </c>
-      <c r="Q6" s="43">
+      <c r="Q6" s="42">
         <v>4</v>
       </c>
-      <c r="R6" s="128"/>
-      <c r="S6" s="130"/>
-      <c r="U6" s="125"/>
-      <c r="V6" s="125"/>
-      <c r="W6" s="125"/>
-      <c r="X6" s="125"/>
-      <c r="Y6" s="44">
+      <c r="R6" s="169"/>
+      <c r="S6" s="171"/>
+      <c r="U6" s="166"/>
+      <c r="V6" s="166"/>
+      <c r="W6" s="166"/>
+      <c r="X6" s="166"/>
+      <c r="Y6" s="43">
         <v>1</v>
       </c>
-      <c r="Z6" s="44">
+      <c r="Z6" s="43">
         <v>2</v>
       </c>
-      <c r="AA6" s="44">
+      <c r="AA6" s="43">
         <v>3</v>
       </c>
-      <c r="AB6" s="44">
+      <c r="AB6" s="43">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="17.25" customHeight="1">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="163"/>
       <c r="D7" s="35" t="e">
         <f>IF(#REF!="GRADE-7","FILIPINO7",IF(#REF!="GRADE-8","FILIPINO8",IF(#REF!="GRADE-9","FILIPINO9",IF(#REF!="GRADE-10","FILIPINO10",""))))</f>
         <v>#REF!</v>
@@ -4122,26 +4127,26 @@
       <c r="R7" s="34"/>
       <c r="S7" s="34"/>
       <c r="T7" s="31"/>
-      <c r="U7" s="107" t="s">
+      <c r="U7" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="V7" s="110" t="s">
+      <c r="V7" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="W7" s="111"/>
-      <c r="X7" s="112"/>
-      <c r="Y7" s="119"/>
-      <c r="Z7" s="119"/>
-      <c r="AA7" s="119"/>
-      <c r="AB7" s="119"/>
+      <c r="W7" s="142"/>
+      <c r="X7" s="143"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="136"/>
+      <c r="AB7" s="136"/>
       <c r="AC7" s="22"/>
     </row>
     <row r="8" spans="1:29" ht="17.25" customHeight="1">
-      <c r="A8" s="132" t="s">
+      <c r="A8" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
+      <c r="B8" s="172"/>
+      <c r="C8" s="172"/>
       <c r="D8" s="35" t="e">
         <f>IF(#REF!="GRADE-7","ENGLISH7",IF(#REF!="GRADE-8","ENGLISH8",IF(#REF!="GRADE-9","ENGLISH9",IF(#REF!="GRADE-10","ENGLISH10",""))))</f>
         <v>#REF!</v>
@@ -4189,115 +4194,115 @@
       <c r="R8" s="34"/>
       <c r="S8" s="34"/>
       <c r="T8" s="31"/>
-      <c r="U8" s="108"/>
-      <c r="V8" s="113"/>
-      <c r="W8" s="114"/>
-      <c r="X8" s="115"/>
-      <c r="Y8" s="120"/>
-      <c r="Z8" s="120"/>
-      <c r="AA8" s="120"/>
-      <c r="AB8" s="120"/>
+      <c r="U8" s="119"/>
+      <c r="V8" s="144"/>
+      <c r="W8" s="145"/>
+      <c r="X8" s="146"/>
+      <c r="Y8" s="137"/>
+      <c r="Z8" s="137"/>
+      <c r="AA8" s="137"/>
+      <c r="AB8" s="137"/>
     </row>
     <row r="9" spans="1:29" ht="8.25" customHeight="1">
-      <c r="A9" s="137" t="s">
+      <c r="A9" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="138"/>
-      <c r="C9" s="139"/>
-      <c r="D9" s="133" t="e">
+      <c r="B9" s="158"/>
+      <c r="C9" s="159"/>
+      <c r="D9" s="173" t="e">
         <f>IF(#REF!="GRADE-7","MATHEMATICS7",IF(#REF!="GRADE-8","MATHEMATICS8",IF(#REF!="GRADE-9","MATHEMATICS9",IF(#REF!="GRADE-10","MATHEMATICS10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E9" s="135" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F9" s="135" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G9" s="135" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H9" s="135" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I9" s="135" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J9" s="135" t="e">
+      <c r="E9" s="112" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F9" s="112" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G9" s="112" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H9" s="112" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I9" s="112" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J9" s="112" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K9" s="135" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L9" s="135" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M9" s="135" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N9" s="143"/>
-      <c r="O9" s="143"/>
-      <c r="P9" s="143"/>
-      <c r="Q9" s="143"/>
-      <c r="R9" s="143"/>
-      <c r="S9" s="143"/>
+      <c r="K9" s="112" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L9" s="112" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M9" s="112" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N9" s="139"/>
+      <c r="O9" s="139"/>
+      <c r="P9" s="139"/>
+      <c r="Q9" s="139"/>
+      <c r="R9" s="139"/>
+      <c r="S9" s="139"/>
       <c r="T9" s="31"/>
-      <c r="U9" s="108"/>
-      <c r="V9" s="116"/>
-      <c r="W9" s="117"/>
-      <c r="X9" s="118"/>
-      <c r="Y9" s="121"/>
-      <c r="Z9" s="121"/>
-      <c r="AA9" s="121"/>
-      <c r="AB9" s="121"/>
+      <c r="U9" s="119"/>
+      <c r="V9" s="147"/>
+      <c r="W9" s="148"/>
+      <c r="X9" s="149"/>
+      <c r="Y9" s="138"/>
+      <c r="Z9" s="138"/>
+      <c r="AA9" s="138"/>
+      <c r="AB9" s="138"/>
     </row>
     <row r="10" spans="1:29" ht="6.75" customHeight="1">
-      <c r="A10" s="140"/>
-      <c r="B10" s="141"/>
-      <c r="C10" s="142"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="136"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="136"/>
-      <c r="I10" s="136"/>
-      <c r="J10" s="136"/>
-      <c r="K10" s="136"/>
-      <c r="L10" s="136"/>
-      <c r="M10" s="136"/>
-      <c r="N10" s="144"/>
-      <c r="O10" s="144"/>
-      <c r="P10" s="144"/>
-      <c r="Q10" s="144"/>
-      <c r="R10" s="144"/>
-      <c r="S10" s="144"/>
+      <c r="A10" s="160"/>
+      <c r="B10" s="161"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="174"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="113"/>
+      <c r="K10" s="113"/>
+      <c r="L10" s="113"/>
+      <c r="M10" s="113"/>
+      <c r="N10" s="140"/>
+      <c r="O10" s="140"/>
+      <c r="P10" s="140"/>
+      <c r="Q10" s="140"/>
+      <c r="R10" s="140"/>
+      <c r="S10" s="140"/>
       <c r="T10" s="31"/>
-      <c r="U10" s="108"/>
-      <c r="V10" s="110" t="s">
+      <c r="U10" s="119"/>
+      <c r="V10" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="W10" s="111"/>
-      <c r="X10" s="112"/>
-      <c r="Y10" s="131"/>
-      <c r="Z10" s="131"/>
-      <c r="AA10" s="131"/>
-      <c r="AB10" s="131"/>
+      <c r="W10" s="142"/>
+      <c r="X10" s="143"/>
+      <c r="Y10" s="117"/>
+      <c r="Z10" s="117"/>
+      <c r="AA10" s="117"/>
+      <c r="AB10" s="117"/>
     </row>
     <row r="11" spans="1:29" ht="17.25" customHeight="1">
-      <c r="A11" s="132" t="s">
+      <c r="A11" s="172" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="132"/>
-      <c r="C11" s="132"/>
+      <c r="B11" s="172"/>
+      <c r="C11" s="172"/>
       <c r="D11" s="35" t="e">
         <f>IF(#REF!="GRADE-7","SCIENCE7",IF(#REF!="GRADE-8","SCIENCE8",IF(#REF!="GRADE-9","SCIENCE9",IF(#REF!="GRADE-10","SCIENCE10",""))))</f>
         <v>#REF!</v>
@@ -4345,21 +4350,21 @@
       <c r="R11" s="34"/>
       <c r="S11" s="34"/>
       <c r="T11" s="31"/>
-      <c r="U11" s="108"/>
-      <c r="V11" s="113"/>
-      <c r="W11" s="114"/>
-      <c r="X11" s="115"/>
-      <c r="Y11" s="131"/>
-      <c r="Z11" s="131"/>
-      <c r="AA11" s="131"/>
-      <c r="AB11" s="131"/>
+      <c r="U11" s="119"/>
+      <c r="V11" s="144"/>
+      <c r="W11" s="145"/>
+      <c r="X11" s="146"/>
+      <c r="Y11" s="117"/>
+      <c r="Z11" s="117"/>
+      <c r="AA11" s="117"/>
+      <c r="AB11" s="117"/>
     </row>
     <row r="12" spans="1:29" ht="20.25" customHeight="1">
-      <c r="A12" s="132" t="s">
+      <c r="A12" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
+      <c r="B12" s="172"/>
+      <c r="C12" s="172"/>
       <c r="D12" s="35" t="e">
         <f>IF(#REF!="GRADE-7","AP7",IF(#REF!="GRADE-8","AP8",IF(#REF!="GRADE-9","AP9",IF(#REF!="GRADE-10","AP10",""))))</f>
         <v>#REF!</v>
@@ -4407,245 +4412,245 @@
       <c r="R12" s="34"/>
       <c r="S12" s="34"/>
       <c r="T12" s="31"/>
-      <c r="U12" s="109"/>
-      <c r="V12" s="116"/>
-      <c r="W12" s="117"/>
-      <c r="X12" s="118"/>
-      <c r="Y12" s="131"/>
-      <c r="Z12" s="131"/>
-      <c r="AA12" s="131"/>
-      <c r="AB12" s="131"/>
+      <c r="U12" s="120"/>
+      <c r="V12" s="147"/>
+      <c r="W12" s="148"/>
+      <c r="X12" s="149"/>
+      <c r="Y12" s="117"/>
+      <c r="Z12" s="117"/>
+      <c r="AA12" s="117"/>
+      <c r="AB12" s="117"/>
     </row>
     <row r="13" spans="1:29" ht="16.5" customHeight="1">
-      <c r="A13" s="160" t="s">
+      <c r="A13" s="155" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="160"/>
-      <c r="C13" s="145"/>
-      <c r="D13" s="107" t="e">
+      <c r="B13" s="155"/>
+      <c r="C13" s="150"/>
+      <c r="D13" s="118" t="e">
         <f>IF(#REF!="GRADE-7","ESP7",IF(#REF!="GRADE-8","ESP8",IF(#REF!="GRADE-9","ESP9",IF(#REF!="GRADE-10","ESP10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E13" s="156" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F13" s="156" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G13" s="156" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H13" s="156" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I13" s="156" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="156" t="e">
+      <c r="E13" s="114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F13" s="114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G13" s="114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H13" s="114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I13" s="114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J13" s="114" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K13" s="156" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L13" s="156" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M13" s="156" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N13" s="161"/>
-      <c r="O13" s="161"/>
-      <c r="P13" s="161"/>
-      <c r="Q13" s="161"/>
-      <c r="R13" s="161"/>
-      <c r="S13" s="143"/>
-      <c r="U13" s="107" t="s">
+      <c r="K13" s="114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L13" s="114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M13" s="114" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N13" s="116"/>
+      <c r="O13" s="116"/>
+      <c r="P13" s="116"/>
+      <c r="Q13" s="116"/>
+      <c r="R13" s="116"/>
+      <c r="S13" s="139"/>
+      <c r="U13" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="V13" s="148" t="s">
+      <c r="V13" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="W13" s="149"/>
-      <c r="X13" s="150"/>
-      <c r="Y13" s="119"/>
-      <c r="Z13" s="119"/>
-      <c r="AA13" s="119"/>
-      <c r="AB13" s="119"/>
+      <c r="W13" s="128"/>
+      <c r="X13" s="129"/>
+      <c r="Y13" s="136"/>
+      <c r="Z13" s="136"/>
+      <c r="AA13" s="136"/>
+      <c r="AB13" s="136"/>
     </row>
     <row r="14" spans="1:29" ht="20.25" customHeight="1">
-      <c r="A14" s="160"/>
-      <c r="B14" s="160"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="157"/>
-      <c r="F14" s="157"/>
-      <c r="G14" s="157"/>
-      <c r="H14" s="157"/>
-      <c r="I14" s="157"/>
-      <c r="J14" s="157"/>
-      <c r="K14" s="157"/>
-      <c r="L14" s="157"/>
-      <c r="M14" s="157"/>
-      <c r="N14" s="161"/>
-      <c r="O14" s="161"/>
-      <c r="P14" s="161"/>
-      <c r="Q14" s="161"/>
-      <c r="R14" s="161"/>
-      <c r="S14" s="144"/>
-      <c r="U14" s="108"/>
-      <c r="V14" s="169"/>
-      <c r="W14" s="170"/>
-      <c r="X14" s="171"/>
-      <c r="Y14" s="120"/>
-      <c r="Z14" s="120"/>
-      <c r="AA14" s="120"/>
-      <c r="AB14" s="120"/>
+      <c r="A14" s="155"/>
+      <c r="B14" s="155"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="115"/>
+      <c r="I14" s="115"/>
+      <c r="J14" s="115"/>
+      <c r="K14" s="115"/>
+      <c r="L14" s="115"/>
+      <c r="M14" s="115"/>
+      <c r="N14" s="116"/>
+      <c r="O14" s="116"/>
+      <c r="P14" s="116"/>
+      <c r="Q14" s="116"/>
+      <c r="R14" s="116"/>
+      <c r="S14" s="140"/>
+      <c r="U14" s="119"/>
+      <c r="V14" s="130"/>
+      <c r="W14" s="131"/>
+      <c r="X14" s="132"/>
+      <c r="Y14" s="137"/>
+      <c r="Z14" s="137"/>
+      <c r="AA14" s="137"/>
+      <c r="AB14" s="137"/>
     </row>
     <row r="15" spans="1:29" ht="13.5" customHeight="1">
-      <c r="A15" s="162" t="s">
+      <c r="A15" s="156" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="162"/>
-      <c r="C15" s="162"/>
-      <c r="D15" s="154" t="e">
+      <c r="B15" s="156"/>
+      <c r="C15" s="156"/>
+      <c r="D15" s="153" t="e">
         <f>IF(#REF!="GRADE-7","TLE7",IF(#REF!="GRADE-8","TLE8",IF(#REF!="GRADE-9","TLE9",IF(#REF!="GRADE-10","TLE10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E15" s="158" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F15" s="158" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G15" s="158" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H15" s="158" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I15" s="158" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J15" s="158" t="e">
+      <c r="E15" s="106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F15" s="106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G15" s="106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H15" s="106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I15" s="106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J15" s="106" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K15" s="158" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L15" s="158" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M15" s="158" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N15" s="161"/>
-      <c r="O15" s="161"/>
-      <c r="P15" s="161"/>
-      <c r="Q15" s="161"/>
-      <c r="R15" s="161"/>
-      <c r="S15" s="143"/>
-      <c r="U15" s="108"/>
-      <c r="V15" s="151"/>
-      <c r="W15" s="152"/>
-      <c r="X15" s="153"/>
-      <c r="Y15" s="121"/>
-      <c r="Z15" s="121"/>
-      <c r="AA15" s="121"/>
-      <c r="AB15" s="121"/>
+      <c r="K15" s="106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L15" s="106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M15" s="106" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N15" s="116"/>
+      <c r="O15" s="116"/>
+      <c r="P15" s="116"/>
+      <c r="Q15" s="116"/>
+      <c r="R15" s="116"/>
+      <c r="S15" s="139"/>
+      <c r="U15" s="119"/>
+      <c r="V15" s="133"/>
+      <c r="W15" s="134"/>
+      <c r="X15" s="135"/>
+      <c r="Y15" s="138"/>
+      <c r="Z15" s="138"/>
+      <c r="AA15" s="138"/>
+      <c r="AB15" s="138"/>
     </row>
     <row r="16" spans="1:29" ht="16.5" customHeight="1">
-      <c r="A16" s="162"/>
-      <c r="B16" s="162"/>
-      <c r="C16" s="162"/>
-      <c r="D16" s="155"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
-      <c r="M16" s="159"/>
-      <c r="N16" s="161"/>
-      <c r="O16" s="161"/>
-      <c r="P16" s="161"/>
-      <c r="Q16" s="161"/>
-      <c r="R16" s="161"/>
-      <c r="S16" s="144"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="108"/>
-      <c r="V16" s="148" t="s">
+      <c r="A16" s="156"/>
+      <c r="B16" s="156"/>
+      <c r="C16" s="156"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="107"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="107"/>
+      <c r="N16" s="116"/>
+      <c r="O16" s="116"/>
+      <c r="P16" s="116"/>
+      <c r="Q16" s="116"/>
+      <c r="R16" s="116"/>
+      <c r="S16" s="140"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="119"/>
+      <c r="V16" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="W16" s="149"/>
-      <c r="X16" s="150"/>
-      <c r="Y16" s="131"/>
-      <c r="Z16" s="131"/>
-      <c r="AA16" s="131"/>
-      <c r="AB16" s="131"/>
+      <c r="W16" s="128"/>
+      <c r="X16" s="129"/>
+      <c r="Y16" s="117"/>
+      <c r="Z16" s="117"/>
+      <c r="AA16" s="117"/>
+      <c r="AB16" s="117"/>
     </row>
     <row r="17" spans="1:28" ht="19.5" customHeight="1">
-      <c r="A17" s="145" t="s">
+      <c r="A17" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="147"/>
-      <c r="D17" s="38" t="e">
+      <c r="B17" s="151"/>
+      <c r="C17" s="152"/>
+      <c r="D17" s="37" t="e">
         <f>IF(#REF!="GRADE-7","MAPEH7",IF(#REF!="GRADE-8","MAPEH8",IF(#REF!="GRADE-9","MAPEH9",IF(#REF!="GRADE-10","MAPEH10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E17" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F17" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G17" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H17" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I17" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J17" s="38" t="e">
+      <c r="E17" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F17" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G17" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H17" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I17" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J17" s="37" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K17" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L17" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M17" s="38" t="e">
+      <c r="K17" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L17" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M17" s="37" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -4654,60 +4659,60 @@
       <c r="P17" s="34"/>
       <c r="Q17" s="34"/>
       <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="109"/>
-      <c r="V17" s="151"/>
-      <c r="W17" s="152"/>
-      <c r="X17" s="153"/>
-      <c r="Y17" s="131"/>
-      <c r="Z17" s="131"/>
-      <c r="AA17" s="131"/>
-      <c r="AB17" s="131"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="120"/>
+      <c r="V17" s="133"/>
+      <c r="W17" s="134"/>
+      <c r="X17" s="135"/>
+      <c r="Y17" s="117"/>
+      <c r="Z17" s="117"/>
+      <c r="AA17" s="117"/>
+      <c r="AB17" s="117"/>
     </row>
     <row r="18" spans="1:28" ht="17.25" customHeight="1">
-      <c r="A18" s="39"/>
-      <c r="B18" s="172" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="173"/>
-      <c r="D18" s="40" t="e">
+      <c r="C18" s="109"/>
+      <c r="D18" s="39" t="e">
         <f>IF(#REF!="GRADE-7","MUSIC7",IF(#REF!="GRADE-8","MUSIC8",IF(#REF!="GRADE-9","MUSIC9",IF(#REF!="GRADE-10","MUSIC10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E18" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F18" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G18" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H18" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I18" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J18" s="40" t="e">
+      <c r="E18" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F18" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G18" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H18" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I18" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J18" s="39" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K18" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L18" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M18" s="40" t="e">
+      <c r="K18" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L18" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M18" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -4715,65 +4720,65 @@
       <c r="O18" s="34"/>
       <c r="P18" s="34"/>
       <c r="Q18" s="34"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="107" t="s">
+      <c r="R18" s="175"/>
+      <c r="S18" s="175"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="V18" s="163" t="s">
+      <c r="V18" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="W18" s="164"/>
-      <c r="X18" s="165"/>
-      <c r="Y18" s="131"/>
-      <c r="Z18" s="131"/>
-      <c r="AA18" s="131"/>
-      <c r="AB18" s="131"/>
+      <c r="W18" s="122"/>
+      <c r="X18" s="123"/>
+      <c r="Y18" s="117"/>
+      <c r="Z18" s="117"/>
+      <c r="AA18" s="117"/>
+      <c r="AB18" s="117"/>
     </row>
     <row r="19" spans="1:28" ht="23.25" customHeight="1">
-      <c r="A19" s="39"/>
-      <c r="B19" s="172" t="s">
+      <c r="A19" s="38"/>
+      <c r="B19" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="173"/>
-      <c r="D19" s="40" t="e">
+      <c r="C19" s="109"/>
+      <c r="D19" s="39" t="e">
         <f>IF(#REF!="GRADE-7","ARTS7",IF(#REF!="GRADE-8","ARTS8",IF(#REF!="GRADE-9","ARTS9",IF(#REF!="GRADE-10","ARTS10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E19" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F19" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G19" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H19" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I19" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J19" s="40" t="e">
+      <c r="E19" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F19" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G19" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H19" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I19" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J19" s="39" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K19" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L19" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M19" s="40" t="e">
+      <c r="K19" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L19" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M19" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -4781,61 +4786,61 @@
       <c r="O19" s="34"/>
       <c r="P19" s="34"/>
       <c r="Q19" s="34"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="37"/>
-      <c r="U19" s="109"/>
-      <c r="V19" s="166"/>
-      <c r="W19" s="167"/>
-      <c r="X19" s="168"/>
-      <c r="Y19" s="131"/>
-      <c r="Z19" s="131"/>
-      <c r="AA19" s="131"/>
-      <c r="AB19" s="131"/>
+      <c r="R19" s="175"/>
+      <c r="S19" s="175"/>
+      <c r="T19" s="36"/>
+      <c r="U19" s="120"/>
+      <c r="V19" s="124"/>
+      <c r="W19" s="125"/>
+      <c r="X19" s="126"/>
+      <c r="Y19" s="117"/>
+      <c r="Z19" s="117"/>
+      <c r="AA19" s="117"/>
+      <c r="AB19" s="117"/>
     </row>
     <row r="20" spans="1:28" ht="19.5" customHeight="1">
-      <c r="A20" s="41"/>
-      <c r="B20" s="172" t="s">
+      <c r="A20" s="40"/>
+      <c r="B20" s="108" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="173"/>
-      <c r="D20" s="40" t="e">
+      <c r="C20" s="109"/>
+      <c r="D20" s="39" t="e">
         <f>IF(#REF!="GRADE-7","PE7",IF(#REF!="GRADE-8","PE8",IF(#REF!="GRADE-9","PE9",IF(#REF!="GRADE-10","PE10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E20" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F20" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G20" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H20" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I20" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J20" s="40" t="e">
+      <c r="E20" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F20" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G20" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H20" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I20" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J20" s="39" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K20" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L20" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M20" s="40" t="e">
+      <c r="K20" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L20" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M20" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -4843,65 +4848,65 @@
       <c r="O20" s="34"/>
       <c r="P20" s="34"/>
       <c r="Q20" s="34"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="107" t="s">
+      <c r="R20" s="175"/>
+      <c r="S20" s="175"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="V20" s="163" t="s">
+      <c r="V20" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="W20" s="164"/>
-      <c r="X20" s="165"/>
-      <c r="Y20" s="131"/>
-      <c r="Z20" s="131"/>
-      <c r="AA20" s="131"/>
-      <c r="AB20" s="131"/>
+      <c r="W20" s="122"/>
+      <c r="X20" s="123"/>
+      <c r="Y20" s="117"/>
+      <c r="Z20" s="117"/>
+      <c r="AA20" s="117"/>
+      <c r="AB20" s="117"/>
     </row>
     <row r="21" spans="1:28" ht="33" customHeight="1">
-      <c r="A21" s="41"/>
-      <c r="B21" s="172" t="s">
+      <c r="A21" s="40"/>
+      <c r="B21" s="108" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="173"/>
-      <c r="D21" s="40" t="e">
+      <c r="C21" s="109"/>
+      <c r="D21" s="39" t="e">
         <f>IF(#REF!="GRADE-7","HEALTH7",IF(#REF!="GRADE-8","HEALTH8",IF(#REF!="GRADE-9","HEALTH9",IF(#REF!="GRADE-10","HEALTH10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="E21" s="38" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F21" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G21" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H21" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I21" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J21" s="40" t="e">
+      <c r="E21" s="37" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F21" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G21" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H21" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I21" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J21" s="39" t="e">
         <f>IF(#REF!="GRADE-7","7",IF(#REF!="GRADE-8","8",IF(#REF!="GRADE-9","9",IF(#REF!="GRADE-10","10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="K21" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L21" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M21" s="40" t="e">
+      <c r="K21" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L21" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M21" s="39" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
@@ -4909,80 +4914,80 @@
       <c r="O21" s="34"/>
       <c r="P21" s="34"/>
       <c r="Q21" s="34"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="108"/>
-      <c r="V21" s="166"/>
-      <c r="W21" s="167"/>
-      <c r="X21" s="168"/>
-      <c r="Y21" s="131"/>
-      <c r="Z21" s="131"/>
-      <c r="AA21" s="131"/>
-      <c r="AB21" s="131"/>
+      <c r="R21" s="175"/>
+      <c r="S21" s="175"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="119"/>
+      <c r="V21" s="124"/>
+      <c r="W21" s="125"/>
+      <c r="X21" s="126"/>
+      <c r="Y21" s="117"/>
+      <c r="Z21" s="117"/>
+      <c r="AA21" s="117"/>
+      <c r="AB21" s="117"/>
     </row>
     <row r="22" spans="1:28" ht="27" customHeight="1">
       <c r="D22" s="32" t="e">
         <f>IF(#REF!="GRADE-7","GEN7",IF(#REF!="GRADE-8","GEN8",IF(#REF!="GRADE-9","GEN9",IF(#REF!="GRADE-10","GEN10",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="N22" s="174" t="s">
+      <c r="N22" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="O22" s="174"/>
-      <c r="P22" s="174"/>
-      <c r="Q22" s="174"/>
-      <c r="R22" s="42"/>
-      <c r="U22" s="108"/>
-      <c r="V22" s="163" t="s">
+      <c r="O22" s="111"/>
+      <c r="P22" s="111"/>
+      <c r="Q22" s="111"/>
+      <c r="R22" s="41"/>
+      <c r="U22" s="119"/>
+      <c r="V22" s="121" t="s">
         <v>33</v>
       </c>
-      <c r="W22" s="164"/>
-      <c r="X22" s="165"/>
-      <c r="Y22" s="131"/>
-      <c r="Z22" s="131"/>
-      <c r="AA22" s="131"/>
-      <c r="AB22" s="131"/>
+      <c r="W22" s="122"/>
+      <c r="X22" s="123"/>
+      <c r="Y22" s="117"/>
+      <c r="Z22" s="117"/>
+      <c r="AA22" s="117"/>
+      <c r="AB22" s="117"/>
     </row>
     <row r="23" spans="1:28" ht="27" customHeight="1">
-      <c r="U23" s="109"/>
-      <c r="V23" s="166"/>
-      <c r="W23" s="167"/>
-      <c r="X23" s="168"/>
-      <c r="Y23" s="131"/>
-      <c r="Z23" s="131"/>
-      <c r="AA23" s="131"/>
-      <c r="AB23" s="131"/>
+      <c r="U23" s="120"/>
+      <c r="V23" s="124"/>
+      <c r="W23" s="125"/>
+      <c r="X23" s="126"/>
+      <c r="Y23" s="117"/>
+      <c r="Z23" s="117"/>
+      <c r="AA23" s="117"/>
+      <c r="AB23" s="117"/>
     </row>
     <row r="24" spans="1:28" ht="15" customHeight="1">
       <c r="A24" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N24" s="122" t="s">
+      <c r="N24" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="O24" s="122"/>
-      <c r="P24" s="122"/>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122" t="s">
+      <c r="O24" s="110"/>
+      <c r="P24" s="110"/>
+      <c r="Q24" s="110"/>
+      <c r="R24" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="S24" s="122"/>
+      <c r="S24" s="110"/>
     </row>
     <row r="25" spans="1:28" ht="15" customHeight="1">
       <c r="A25" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="N25" s="56" t="s">
+      <c r="N25" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="56" t="s">
+      <c r="O25" s="103"/>
+      <c r="P25" s="103"/>
+      <c r="Q25" s="103"/>
+      <c r="R25" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="S25" s="56"/>
+      <c r="S25" s="103"/>
       <c r="V25" s="22" t="s">
         <v>39</v>
       </c>
@@ -4994,16 +4999,16 @@
       <c r="A26" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="N26" s="56" t="s">
+      <c r="N26" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="O26" s="56"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="56" t="s">
+      <c r="O26" s="103"/>
+      <c r="P26" s="103"/>
+      <c r="Q26" s="103"/>
+      <c r="R26" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="S26" s="56"/>
+      <c r="S26" s="103"/>
       <c r="V26" s="31" t="s">
         <v>43</v>
       </c>
@@ -5015,16 +5020,16 @@
       <c r="A27" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="N27" s="56" t="s">
+      <c r="N27" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="56" t="s">
+      <c r="O27" s="103"/>
+      <c r="P27" s="103"/>
+      <c r="Q27" s="103"/>
+      <c r="R27" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="S27" s="56"/>
+      <c r="S27" s="103"/>
       <c r="V27" s="31" t="s">
         <v>47</v>
       </c>
@@ -5036,16 +5041,16 @@
       <c r="A28" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="N28" s="56" t="s">
+      <c r="N28" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56" t="s">
+      <c r="O28" s="103"/>
+      <c r="P28" s="103"/>
+      <c r="Q28" s="103"/>
+      <c r="R28" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="S28" s="56"/>
+      <c r="S28" s="103"/>
       <c r="V28" s="31" t="s">
         <v>51</v>
       </c>
@@ -5057,16 +5062,16 @@
       <c r="A29" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="N29" s="56" t="s">
+      <c r="N29" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56" t="s">
+      <c r="O29" s="103"/>
+      <c r="P29" s="103"/>
+      <c r="Q29" s="103"/>
+      <c r="R29" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="S29" s="56"/>
+      <c r="S29" s="103"/>
       <c r="V29" s="31" t="s">
         <v>56</v>
       </c>
@@ -5076,6 +5081,103 @@
     </row>
   </sheetData>
   <mergeCells count="121">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="U7:U12"/>
+    <mergeCell ref="V7:X9"/>
+    <mergeCell ref="Y7:Y9"/>
+    <mergeCell ref="Z7:Z9"/>
+    <mergeCell ref="AA7:AA9"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="A5:C6"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:X6"/>
+    <mergeCell ref="Y5:AB5"/>
+    <mergeCell ref="AB10:AB12"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="AA10:AA12"/>
+    <mergeCell ref="AB7:AB9"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="Y10:Y12"/>
+    <mergeCell ref="Z10:Z12"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A9:C10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="V10:X12"/>
+    <mergeCell ref="Z13:Z15"/>
+    <mergeCell ref="AA13:AA15"/>
+    <mergeCell ref="AB13:AB15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="V16:X17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="Z16:Z17"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="A13:C14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="A15:C16"/>
+    <mergeCell ref="Z18:Z19"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="AA18:AA19"/>
+    <mergeCell ref="AB18:AB19"/>
+    <mergeCell ref="U20:U23"/>
+    <mergeCell ref="V20:X21"/>
+    <mergeCell ref="Y20:Y21"/>
+    <mergeCell ref="Z20:Z21"/>
+    <mergeCell ref="AA20:AA21"/>
+    <mergeCell ref="AB20:AB21"/>
+    <mergeCell ref="V22:X23"/>
+    <mergeCell ref="Y22:Y23"/>
+    <mergeCell ref="Z22:Z23"/>
+    <mergeCell ref="AA22:AA23"/>
+    <mergeCell ref="AB22:AB23"/>
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="U13:U17"/>
+    <mergeCell ref="V13:X15"/>
+    <mergeCell ref="Y13:Y15"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="V18:X19"/>
+    <mergeCell ref="Y18:Y19"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
@@ -5100,103 +5202,6 @@
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="Z18:Z19"/>
-    <mergeCell ref="AA16:AA17"/>
-    <mergeCell ref="AA18:AA19"/>
-    <mergeCell ref="AB18:AB19"/>
-    <mergeCell ref="U20:U23"/>
-    <mergeCell ref="V20:X21"/>
-    <mergeCell ref="Y20:Y21"/>
-    <mergeCell ref="Z20:Z21"/>
-    <mergeCell ref="AA20:AA21"/>
-    <mergeCell ref="AB20:AB21"/>
-    <mergeCell ref="V22:X23"/>
-    <mergeCell ref="Y22:Y23"/>
-    <mergeCell ref="Z22:Z23"/>
-    <mergeCell ref="AA22:AA23"/>
-    <mergeCell ref="AB22:AB23"/>
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="U13:U17"/>
-    <mergeCell ref="V13:X15"/>
-    <mergeCell ref="Y13:Y15"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="V18:X19"/>
-    <mergeCell ref="Y18:Y19"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="V10:X12"/>
-    <mergeCell ref="Z13:Z15"/>
-    <mergeCell ref="AA13:AA15"/>
-    <mergeCell ref="AB13:AB15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="V16:X17"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="Z16:Z17"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="A13:C14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="A15:C16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A9:C10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="U7:U12"/>
-    <mergeCell ref="V7:X9"/>
-    <mergeCell ref="Y7:Y9"/>
-    <mergeCell ref="Z7:Z9"/>
-    <mergeCell ref="AA7:AA9"/>
-    <mergeCell ref="A3:S3"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="A5:C6"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:X6"/>
-    <mergeCell ref="Y5:AB5"/>
-    <mergeCell ref="AB10:AB12"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="AA10:AA12"/>
-    <mergeCell ref="AB7:AB9"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="Y10:Y12"/>
-    <mergeCell ref="Z10:Z12"/>
-    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>